<commit_message>
Italy and #8 done
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/countries/Italy_1.xlsx
+++ b/a-place-for-salvador-allende/countries/Italy_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/countries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="11_0835A3F0F613C8A64DC3FD8AC9E9C82E4FD6E783" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B218470C-4AA7-4B19-BB0A-24072E4B14B7}"/>
+  <xr:revisionPtr revIDLastSave="281" documentId="11_0835A3F0F613C8A64DC3FD8AC9E9C82E4FD6E783" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2314C987-F299-4E9B-8C2C-92AB9E6E9207}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="169">
   <si>
     <t>id</t>
   </si>
@@ -536,6 +536,23 @@
   </si>
   <si>
     <t>Crocetta</t>
+  </si>
+  <si>
+    <t>Molassana</t>
+  </si>
+  <si>
+    <t>Piazza Salvador Allende
+Politico e medico cileno 1908-1973</t>
+  </si>
+  <si>
+    <t>Salvator Allende
+Martire antifascista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molassana
+Via Salvador Allende
+Uomo politico cileno. 1908 - 1973
+</t>
   </si>
 </sst>
 </file>
@@ -952,10 +969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Y22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,7 +1114,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>224</v>
       </c>
@@ -1965,6 +1983,9 @@
       <c r="H17" t="s">
         <v>139</v>
       </c>
+      <c r="I17" t="s">
+        <v>165</v>
+      </c>
       <c r="K17">
         <v>16138</v>
       </c>
@@ -1985,6 +2006,12 @@
       </c>
       <c r="Q17" t="s">
         <v>63</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="S17" t="s">
+        <v>83</v>
       </c>
       <c r="V17">
         <v>1</v>
@@ -2172,6 +2199,12 @@
       <c r="Q20" t="s">
         <v>63</v>
       </c>
+      <c r="R20" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="S20" t="s">
+        <v>83</v>
+      </c>
       <c r="V20">
         <v>1</v>
       </c>
@@ -2299,6 +2332,12 @@
       <c r="Q22" t="s">
         <v>63</v>
       </c>
+      <c r="R22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="S22" t="s">
+        <v>83</v>
+      </c>
       <c r="V22">
         <v>1</v>
       </c>
@@ -2313,7 +2352,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y22" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Y22" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="23">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="Y2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="W3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>